<commit_message>
Update Valkyrie V2 HT100 BOM Beta.xlsx
</commit_message>
<xml_diff>
--- a/V2 BETA/BOM/Valkyrie V2 HT100 BOM Beta.xlsx
+++ b/V2 BETA/BOM/Valkyrie V2 HT100 BOM Beta.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3837cd5b4a1a02ac/Document Library/GitHub/Project-Valkyrie/V2 BETA/BOM/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="223" documentId="8_{5107759B-8870-48A8-933E-C4A7F6F41B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8C202E79-49ED-46B3-B55A-A32005330312}"/>
+  <xr:revisionPtr revIDLastSave="230" documentId="8_{5107759B-8870-48A8-933E-C4A7F6F41B8D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{75F28898-E707-4D07-8866-73164ED7823E}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-45" windowWidth="29040" windowHeight="16440" activeTab="11" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -54,7 +54,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1249" uniqueCount="691">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1252" uniqueCount="694">
   <si>
     <t>Type - System</t>
   </si>
@@ -2108,7 +2108,7 @@
     <t xml:space="preserve">EPDM foam </t>
   </si>
   <si>
-    <t>3M</t>
+    <t>5M</t>
   </si>
   <si>
     <t>Door seal / Dry Box</t>
@@ -2120,6 +2120,9 @@
     <t xml:space="preserve">Square </t>
   </si>
   <si>
+    <t>Engineers square</t>
+  </si>
+  <si>
     <t xml:space="preserve">Allen keys </t>
   </si>
   <si>
@@ -2129,7 +2132,10 @@
     <t xml:space="preserve">G or F clamp </t>
   </si>
   <si>
-    <t>Spanner  AF</t>
+    <t xml:space="preserve">gust for putting the frame together </t>
+  </si>
+  <si>
+    <t>Spanner  AF 7mm,</t>
   </si>
   <si>
     <t>Drill bits ,M5</t>
@@ -2145,6 +2151,9 @@
   </si>
   <si>
     <t xml:space="preserve">calipers </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Good choice Shahe </t>
   </si>
 </sst>
 </file>
@@ -11001,14 +11010,14 @@
   <dimension ref="A1:E12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
     <col min="1" max="1" width="42.7109375" customWidth="1"/>
     <col min="2" max="2" width="20.42578125" customWidth="1"/>
-    <col min="3" max="3" width="19.140625" customWidth="1"/>
+    <col min="3" max="3" width="32.85546875" customWidth="1"/>
     <col min="4" max="4" width="19.42578125" customWidth="1"/>
     <col min="5" max="5" width="34.42578125" customWidth="1"/>
   </cols>
@@ -11048,50 +11057,59 @@
       <c r="A3" t="s">
         <v>681</v>
       </c>
+      <c r="C3" t="s">
+        <v>682</v>
+      </c>
     </row>
     <row r="4" spans="1:5">
       <c r="A4" t="s">
-        <v>682</v>
+        <v>683</v>
       </c>
     </row>
     <row r="5" spans="1:5">
       <c r="A5" t="s">
-        <v>683</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5">
+        <v>684</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" ht="16.5" customHeight="1">
       <c r="A6" t="s">
-        <v>684</v>
+        <v>685</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>686</v>
       </c>
     </row>
     <row r="7" spans="1:5">
       <c r="A7" t="s">
-        <v>685</v>
+        <v>687</v>
       </c>
     </row>
     <row r="8" spans="1:5">
       <c r="A8" t="s">
-        <v>686</v>
+        <v>688</v>
       </c>
     </row>
     <row r="9" spans="1:5">
       <c r="A9" t="s">
-        <v>687</v>
+        <v>689</v>
       </c>
     </row>
     <row r="10" spans="1:5" ht="14.25" customHeight="1">
       <c r="A10" s="4" t="s">
-        <v>688</v>
+        <v>690</v>
       </c>
     </row>
     <row r="11" spans="1:5">
       <c r="A11" t="s">
-        <v>689</v>
+        <v>691</v>
       </c>
     </row>
     <row r="12" spans="1:5">
       <c r="A12" t="s">
-        <v>690</v>
+        <v>692</v>
+      </c>
+      <c r="C12" t="s">
+        <v>693</v>
       </c>
     </row>
   </sheetData>

</xml_diff>